<commit_message>
Fine test hybrid no radiant
</commit_message>
<xml_diff>
--- a/Modello/nuovi modelli/Input-Output.xlsx
+++ b/Modello/nuovi modelli/Input-Output.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test-1" sheetId="3" r:id="rId1"/>
@@ -31,12 +31,12 @@
     <definedName name="Output6">'Test-2-k'!$B$4:$AL$6</definedName>
     <definedName name="Output7">'Test-2-R'!$B$4:$AL$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="84">
   <si>
     <t>ATM/CNS provision costs</t>
   </si>
@@ -283,13 +283,19 @@
   <si>
     <t>k</t>
   </si>
+  <si>
+    <t>0.00000001</t>
+  </si>
+  <si>
+    <t>0.0000001</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -447,7 +453,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -543,6 +549,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -578,6 +601,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1352,32 +1392,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="T1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="19" max="19" width="17" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" customWidth="1"/>
-    <col min="22" max="22" width="8.88671875" customWidth="1"/>
-    <col min="25" max="25" width="8.88671875" customWidth="1"/>
-    <col min="27" max="27" width="12.44140625" customWidth="1"/>
-    <col min="29" max="29" width="18.88671875" customWidth="1"/>
-    <col min="30" max="30" width="24.21875" customWidth="1"/>
-    <col min="31" max="31" width="8.88671875" customWidth="1"/>
-    <col min="32" max="32" width="15.6640625" customWidth="1"/>
-    <col min="34" max="34" width="12" customWidth="1"/>
-    <col min="36" max="36" width="19.5546875" customWidth="1"/>
-    <col min="38" max="38" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="258" max="258" width="12.88671875" customWidth="1"/>
     <col min="260" max="260" width="8.88671875" customWidth="1"/>
     <col min="261" max="261" width="15.109375" customWidth="1"/>
@@ -3224,14 +3276,14 @@
       <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="7">
-        <v>0</v>
+      <c r="B6" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="C6" s="6">
         <v>8</v>
       </c>
-      <c r="D6" s="6">
-        <v>0</v>
+      <c r="D6" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="E6" s="6">
         <v>20</v>
@@ -3242,8 +3294,8 @@
       <c r="G6" s="6">
         <v>10</v>
       </c>
-      <c r="H6" s="6">
-        <v>0</v>
+      <c r="H6" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="I6" s="6">
         <v>163</v>
@@ -3278,14 +3330,14 @@
       <c r="S6" s="6">
         <v>1</v>
       </c>
-      <c r="T6" s="6">
-        <v>0</v>
+      <c r="T6" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="U6" s="6">
         <v>24</v>
       </c>
-      <c r="V6" s="6">
-        <v>0</v>
+      <c r="V6" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="W6" s="6">
         <v>61</v>
@@ -3293,14 +3345,14 @@
       <c r="X6" s="6">
         <v>70</v>
       </c>
-      <c r="Y6" s="6">
-        <v>0</v>
+      <c r="Y6" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="Z6" s="6">
         <v>1</v>
       </c>
-      <c r="AA6" s="6">
-        <v>0</v>
+      <c r="AA6" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="AB6" s="6">
         <v>281</v>
@@ -3311,17 +3363,17 @@
       <c r="AD6" s="6">
         <v>240</v>
       </c>
-      <c r="AE6" s="6">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="6">
-        <v>0</v>
+      <c r="AE6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="AG6" s="6">
         <v>547</v>
       </c>
-      <c r="AH6" s="6">
-        <v>0</v>
+      <c r="AH6" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="AI6" s="6">
         <v>120</v>
@@ -3332,8 +3384,8 @@
       <c r="AK6" s="6">
         <v>2</v>
       </c>
-      <c r="AL6" s="6">
-        <v>0</v>
+      <c r="AL6" s="6" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.3">
@@ -3341,6 +3393,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7611,7 +7664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+    <sheetView topLeftCell="AD7" workbookViewId="0">
       <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Test Non Discretional Input
</commit_message>
<xml_diff>
--- a/Modello/nuovi modelli/Input-Output.xlsx
+++ b/Modello/nuovi modelli/Input-Output.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Test-1" sheetId="3" r:id="rId1"/>
@@ -14,8 +14,11 @@
     <sheet name="Test-2-R" sheetId="9" r:id="rId5"/>
     <sheet name="Test-3" sheetId="5" r:id="rId6"/>
     <sheet name="Test-4" sheetId="6" r:id="rId7"/>
+    <sheet name="Test-k-O" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName name="Input_d8">'Test-4'!$B$2:$AL$3</definedName>
+    <definedName name="Input_nd8">'Test-4'!$B$4:$AL$4</definedName>
     <definedName name="Input1">'Test-1'!$B$2:$AL$3</definedName>
     <definedName name="Input2">'Test-2'!$B$2:$AL$3</definedName>
     <definedName name="Input3">'Test-3'!$B$2:$AL$2</definedName>
@@ -23,6 +26,7 @@
     <definedName name="Input5">'Test-2-I'!$B$2:$AL$4</definedName>
     <definedName name="Input6">'Test-2-k'!$B$2:$AL$3</definedName>
     <definedName name="Input7">'Test-2-R'!$B$2:$AL$3</definedName>
+    <definedName name="Input9">'Test-k-O'!$B$2:$AL$3</definedName>
     <definedName name="Output1">'Test-1'!$B$4:$AL$5</definedName>
     <definedName name="Output2">'Test-2'!$B$4:$AL$6</definedName>
     <definedName name="Output3">'Test-3'!$B$3:$AL$4</definedName>
@@ -30,13 +34,15 @@
     <definedName name="Output5">'Test-2-I'!$B$5:$AL$6</definedName>
     <definedName name="Output6">'Test-2-k'!$B$4:$AL$6</definedName>
     <definedName name="Output7">'Test-2-R'!$B$4:$AL$6</definedName>
+    <definedName name="Output8">'Test-4'!$B$5:$AL$6</definedName>
+    <definedName name="Output9">'Test-k-O'!$B$4:$AL$6</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="84">
   <si>
     <t>ATM/CNS provision costs</t>
   </si>
@@ -1392,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="T1" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3401,8 +3407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5397,8 +5403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL10"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection sqref="A1:AL10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7664,7 +7670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL9"/>
   <sheetViews>
-    <sheetView topLeftCell="AD7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
@@ -9110,8 +9116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection sqref="A1:AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9819,4 +9825,988 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AL11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:AL6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL1" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9">
+        <v>18410</v>
+      </c>
+      <c r="C2" s="9">
+        <v>92051</v>
+      </c>
+      <c r="D2" s="9">
+        <v>4480</v>
+      </c>
+      <c r="E2" s="9">
+        <v>150346</v>
+      </c>
+      <c r="F2" s="9">
+        <v>94434</v>
+      </c>
+      <c r="G2" s="9">
+        <v>98393</v>
+      </c>
+      <c r="H2" s="9">
+        <v>69781</v>
+      </c>
+      <c r="I2" s="9">
+        <v>76524</v>
+      </c>
+      <c r="J2" s="9">
+        <v>34084</v>
+      </c>
+      <c r="K2" s="9">
+        <v>829697</v>
+      </c>
+      <c r="L2" s="9">
+        <v>287980</v>
+      </c>
+      <c r="M2" s="9">
+        <v>958920</v>
+      </c>
+      <c r="N2" s="9">
+        <v>14197</v>
+      </c>
+      <c r="O2" s="9">
+        <v>604266</v>
+      </c>
+      <c r="P2" s="9">
+        <v>556266</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>38230</v>
+      </c>
+      <c r="R2" s="9">
+        <v>127715</v>
+      </c>
+      <c r="S2" s="9">
+        <v>74539</v>
+      </c>
+      <c r="T2" s="9">
+        <v>88518</v>
+      </c>
+      <c r="U2" s="9">
+        <v>165810</v>
+      </c>
+      <c r="V2" s="9">
+        <v>17271</v>
+      </c>
+      <c r="W2" s="9">
+        <v>53196</v>
+      </c>
+      <c r="X2" s="9">
+        <v>118407</v>
+      </c>
+      <c r="Y2" s="9">
+        <v>11556</v>
+      </c>
+      <c r="Z2" s="9">
+        <v>10498</v>
+      </c>
+      <c r="AA2" s="9">
+        <v>5817</v>
+      </c>
+      <c r="AB2" s="9">
+        <v>145335</v>
+      </c>
+      <c r="AC2" s="9">
+        <v>595612</v>
+      </c>
+      <c r="AD2" s="9">
+        <v>89408</v>
+      </c>
+      <c r="AE2" s="9">
+        <v>80124</v>
+      </c>
+      <c r="AF2" s="9">
+        <v>20104</v>
+      </c>
+      <c r="AG2" s="9">
+        <v>142617</v>
+      </c>
+      <c r="AH2" s="9">
+        <v>136127</v>
+      </c>
+      <c r="AI2" s="9">
+        <v>188780</v>
+      </c>
+      <c r="AJ2" s="9">
+        <v>26775</v>
+      </c>
+      <c r="AK2" s="9">
+        <v>60420</v>
+      </c>
+      <c r="AL2" s="9">
+        <v>123204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="9">
+        <v>49</v>
+      </c>
+      <c r="C3" s="9">
+        <v>192</v>
+      </c>
+      <c r="D3" s="9">
+        <v>82</v>
+      </c>
+      <c r="E3" s="9">
+        <v>291</v>
+      </c>
+      <c r="F3" s="9">
+        <v>407</v>
+      </c>
+      <c r="G3" s="9">
+        <v>232</v>
+      </c>
+      <c r="H3" s="9">
+        <v>248</v>
+      </c>
+      <c r="I3" s="9">
+        <v>234</v>
+      </c>
+      <c r="J3" s="9">
+        <v>86</v>
+      </c>
+      <c r="K3" s="9">
+        <v>1777</v>
+      </c>
+      <c r="L3" s="9">
+        <v>1120</v>
+      </c>
+      <c r="M3" s="9">
+        <v>2782</v>
+      </c>
+      <c r="N3" s="9">
+        <v>52</v>
+      </c>
+      <c r="O3" s="9">
+        <v>1779</v>
+      </c>
+      <c r="P3" s="9">
+        <v>1414</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>183</v>
+      </c>
+      <c r="R3" s="9">
+        <v>496</v>
+      </c>
+      <c r="S3" s="9">
+        <v>173</v>
+      </c>
+      <c r="T3" s="9">
+        <v>204</v>
+      </c>
+      <c r="U3" s="9">
+        <v>470</v>
+      </c>
+      <c r="V3" s="9">
+        <v>93</v>
+      </c>
+      <c r="W3" s="9">
+        <v>82</v>
+      </c>
+      <c r="X3" s="9">
+        <v>178</v>
+      </c>
+      <c r="Y3" s="9">
+        <v>54</v>
+      </c>
+      <c r="Z3" s="9">
+        <v>65</v>
+      </c>
+      <c r="AA3" s="9">
+        <v>73</v>
+      </c>
+      <c r="AB3" s="9">
+        <v>268</v>
+      </c>
+      <c r="AC3" s="9">
+        <v>1415</v>
+      </c>
+      <c r="AD3" s="9">
+        <v>220</v>
+      </c>
+      <c r="AE3" s="9">
+        <v>208</v>
+      </c>
+      <c r="AF3" s="9">
+        <v>87</v>
+      </c>
+      <c r="AG3" s="9">
+        <v>479</v>
+      </c>
+      <c r="AH3" s="9">
+        <v>448</v>
+      </c>
+      <c r="AI3" s="9">
+        <v>362</v>
+      </c>
+      <c r="AJ3" s="9">
+        <v>91</v>
+      </c>
+      <c r="AK3" s="9">
+        <v>277</v>
+      </c>
+      <c r="AL3" s="9">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="10">
+        <f>B9*B11</f>
+        <v>-49200</v>
+      </c>
+      <c r="C4" s="10">
+        <f>C9*C11</f>
+        <v>-45120</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" ref="D4:AL4" si="0">D9*D11</f>
+        <v>-44040</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" si="0"/>
+        <v>-41760</v>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" si="0"/>
+        <v>-41040</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" si="0"/>
+        <v>-40760</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" si="0"/>
+        <v>-31680</v>
+      </c>
+      <c r="I4" s="10">
+        <f t="shared" si="0"/>
+        <v>-30720</v>
+      </c>
+      <c r="J4" s="10">
+        <f t="shared" si="0"/>
+        <v>-30520</v>
+      </c>
+      <c r="K4" s="10">
+        <f t="shared" si="0"/>
+        <v>-29320</v>
+      </c>
+      <c r="L4" s="10">
+        <f t="shared" si="0"/>
+        <v>-27360</v>
+      </c>
+      <c r="M4" s="10">
+        <f t="shared" si="0"/>
+        <v>-23760</v>
+      </c>
+      <c r="N4" s="10">
+        <f t="shared" si="0"/>
+        <v>-22920</v>
+      </c>
+      <c r="O4" s="10">
+        <f t="shared" si="0"/>
+        <v>-22080</v>
+      </c>
+      <c r="P4" s="10">
+        <f t="shared" si="0"/>
+        <v>-21040</v>
+      </c>
+      <c r="Q4" s="10">
+        <f t="shared" si="0"/>
+        <v>-20440</v>
+      </c>
+      <c r="R4" s="10">
+        <f t="shared" si="0"/>
+        <v>-17120</v>
+      </c>
+      <c r="S4" s="10">
+        <f t="shared" si="0"/>
+        <v>-17040</v>
+      </c>
+      <c r="T4" s="10">
+        <f t="shared" si="0"/>
+        <v>-16840</v>
+      </c>
+      <c r="U4" s="10">
+        <f t="shared" si="0"/>
+        <v>-16079.999999999998</v>
+      </c>
+      <c r="V4" s="10">
+        <f t="shared" si="0"/>
+        <v>-13840</v>
+      </c>
+      <c r="W4" s="10">
+        <f t="shared" si="0"/>
+        <v>-13280</v>
+      </c>
+      <c r="X4" s="10">
+        <f t="shared" si="0"/>
+        <v>-12520</v>
+      </c>
+      <c r="Y4" s="10">
+        <f t="shared" si="0"/>
+        <v>-12520</v>
+      </c>
+      <c r="Z4" s="10">
+        <f t="shared" si="0"/>
+        <v>-11480</v>
+      </c>
+      <c r="AA4" s="10">
+        <f t="shared" si="0"/>
+        <v>-10640</v>
+      </c>
+      <c r="AB4" s="10">
+        <f t="shared" si="0"/>
+        <v>-10400</v>
+      </c>
+      <c r="AC4" s="10">
+        <f t="shared" si="0"/>
+        <v>-10160</v>
+      </c>
+      <c r="AD4" s="10">
+        <f t="shared" si="0"/>
+        <v>-9400</v>
+      </c>
+      <c r="AE4" s="10">
+        <f t="shared" si="0"/>
+        <v>-8760</v>
+      </c>
+      <c r="AF4" s="10">
+        <f t="shared" si="0"/>
+        <v>-8720</v>
+      </c>
+      <c r="AG4" s="10">
+        <f t="shared" si="0"/>
+        <v>-7800</v>
+      </c>
+      <c r="AH4" s="10">
+        <f t="shared" si="0"/>
+        <v>-6560</v>
+      </c>
+      <c r="AI4" s="10">
+        <f t="shared" si="0"/>
+        <v>-6280</v>
+      </c>
+      <c r="AJ4" s="10">
+        <f t="shared" si="0"/>
+        <v>-4640</v>
+      </c>
+      <c r="AK4" s="10">
+        <f t="shared" si="0"/>
+        <v>-3760</v>
+      </c>
+      <c r="AL4" s="10">
+        <f t="shared" si="0"/>
+        <v>-3240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="10">
+        <v>198399</v>
+      </c>
+      <c r="C5" s="10">
+        <v>682563</v>
+      </c>
+      <c r="D5" s="10">
+        <v>50239</v>
+      </c>
+      <c r="E5" s="10">
+        <v>903549</v>
+      </c>
+      <c r="F5" s="10">
+        <v>621113</v>
+      </c>
+      <c r="G5" s="10">
+        <v>563112</v>
+      </c>
+      <c r="H5" s="10">
+        <v>683320</v>
+      </c>
+      <c r="I5" s="10">
+        <v>520874</v>
+      </c>
+      <c r="J5" s="10">
+        <v>304328</v>
+      </c>
+      <c r="K5" s="10">
+        <v>2772617</v>
+      </c>
+      <c r="L5" s="10">
+        <v>1235140</v>
+      </c>
+      <c r="M5" s="10">
+        <v>2845477</v>
+      </c>
+      <c r="N5" s="10">
+        <v>190501</v>
+      </c>
+      <c r="O5" s="10">
+        <v>1681498</v>
+      </c>
+      <c r="P5" s="10">
+        <v>1550608</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>229263</v>
+      </c>
+      <c r="R5" s="10">
+        <v>677777</v>
+      </c>
+      <c r="S5" s="10">
+        <v>717157</v>
+      </c>
+      <c r="T5" s="10">
+        <v>536948</v>
+      </c>
+      <c r="U5" s="10">
+        <v>682995</v>
+      </c>
+      <c r="V5" s="10">
+        <v>240571</v>
+      </c>
+      <c r="W5" s="10">
+        <v>435890</v>
+      </c>
+      <c r="X5" s="10">
+        <v>567805</v>
+      </c>
+      <c r="Y5" s="10">
+        <v>101906</v>
+      </c>
+      <c r="Z5" s="10">
+        <v>146380</v>
+      </c>
+      <c r="AA5" s="10">
+        <v>56298</v>
+      </c>
+      <c r="AB5" s="10">
+        <v>1671185</v>
+      </c>
+      <c r="AC5" s="10">
+        <v>2214690</v>
+      </c>
+      <c r="AD5" s="10">
+        <v>479220</v>
+      </c>
+      <c r="AE5" s="10">
+        <v>632309</v>
+      </c>
+      <c r="AF5" s="10">
+        <v>224039</v>
+      </c>
+      <c r="AG5" s="10">
+        <v>690554</v>
+      </c>
+      <c r="AH5" s="10">
+        <v>598230</v>
+      </c>
+      <c r="AI5" s="10">
+        <v>1164916</v>
+      </c>
+      <c r="AJ5" s="10">
+        <v>273748</v>
+      </c>
+      <c r="AK5" s="10">
+        <v>551569</v>
+      </c>
+      <c r="AL5" s="10">
+        <v>320276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="10">
+        <v>46627</v>
+      </c>
+      <c r="C6" s="10">
+        <v>263155</v>
+      </c>
+      <c r="D6" s="10">
+        <v>18939</v>
+      </c>
+      <c r="E6" s="10">
+        <v>366680</v>
+      </c>
+      <c r="F6" s="10">
+        <v>562617</v>
+      </c>
+      <c r="G6" s="10">
+        <v>205396</v>
+      </c>
+      <c r="H6" s="10">
+        <v>239577</v>
+      </c>
+      <c r="I6" s="10">
+        <v>228444</v>
+      </c>
+      <c r="J6" s="10">
+        <v>162044</v>
+      </c>
+      <c r="K6" s="10">
+        <v>1881337</v>
+      </c>
+      <c r="L6" s="10">
+        <v>1508424</v>
+      </c>
+      <c r="M6" s="10">
+        <v>2639898</v>
+      </c>
+      <c r="N6" s="10">
+        <v>74861</v>
+      </c>
+      <c r="O6" s="10">
+        <v>1609082</v>
+      </c>
+      <c r="P6" s="10">
+        <v>1329980</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>170939</v>
+      </c>
+      <c r="R6" s="10">
+        <v>583639</v>
+      </c>
+      <c r="S6" s="10">
+        <v>237116</v>
+      </c>
+      <c r="T6" s="10">
+        <v>336801</v>
+      </c>
+      <c r="U6" s="10">
+        <v>549703</v>
+      </c>
+      <c r="V6" s="10">
+        <v>92886</v>
+      </c>
+      <c r="W6" s="10">
+        <v>99652</v>
+      </c>
+      <c r="X6" s="10">
+        <v>285969</v>
+      </c>
+      <c r="Y6" s="10">
+        <v>77899</v>
+      </c>
+      <c r="Z6" s="10">
+        <v>27956</v>
+      </c>
+      <c r="AA6" s="10">
+        <v>18273</v>
+      </c>
+      <c r="AB6" s="10">
+        <v>587342</v>
+      </c>
+      <c r="AC6" s="10">
+        <v>1781191</v>
+      </c>
+      <c r="AD6" s="10">
+        <v>399808</v>
+      </c>
+      <c r="AE6" s="10">
+        <v>298402</v>
+      </c>
+      <c r="AF6" s="10">
+        <v>66194</v>
+      </c>
+      <c r="AG6" s="10">
+        <v>493168</v>
+      </c>
+      <c r="AH6" s="10">
+        <v>365642</v>
+      </c>
+      <c r="AI6" s="10">
+        <v>450868</v>
+      </c>
+      <c r="AJ6" s="10">
+        <v>57152</v>
+      </c>
+      <c r="AK6" s="10">
+        <v>229245</v>
+      </c>
+      <c r="AL6" s="10">
+        <v>291335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="C9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="D9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="E9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="F9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="G9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="H9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="I9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="J9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="K9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="L9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="M9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="N9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="O9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="P9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="Q9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="R9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="S9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="T9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="U9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="V9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="W9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="X9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="Y9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="Z9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="AA9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="AB9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="AC9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="AD9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="AE9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="AF9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="AG9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="AH9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="AI9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="AJ9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="AK9" s="15">
+        <v>-4000</v>
+      </c>
+      <c r="AL9" s="15">
+        <v>-4000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="10">
+        <v>12.3</v>
+      </c>
+      <c r="C11" s="10">
+        <v>11.28</v>
+      </c>
+      <c r="D11" s="10">
+        <v>11.01</v>
+      </c>
+      <c r="E11" s="10">
+        <v>10.44</v>
+      </c>
+      <c r="F11" s="10">
+        <v>10.26</v>
+      </c>
+      <c r="G11" s="10">
+        <v>10.19</v>
+      </c>
+      <c r="H11" s="10">
+        <v>7.92</v>
+      </c>
+      <c r="I11" s="10">
+        <v>7.68</v>
+      </c>
+      <c r="J11" s="10">
+        <v>7.63</v>
+      </c>
+      <c r="K11" s="10">
+        <v>7.33</v>
+      </c>
+      <c r="L11" s="10">
+        <v>6.84</v>
+      </c>
+      <c r="M11" s="10">
+        <v>5.94</v>
+      </c>
+      <c r="N11" s="10">
+        <v>5.73</v>
+      </c>
+      <c r="O11" s="10">
+        <v>5.52</v>
+      </c>
+      <c r="P11" s="10">
+        <v>5.26</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="R11" s="10">
+        <v>4.28</v>
+      </c>
+      <c r="S11" s="10">
+        <v>4.26</v>
+      </c>
+      <c r="T11" s="10">
+        <v>4.21</v>
+      </c>
+      <c r="U11" s="10">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="V11" s="10">
+        <v>3.46</v>
+      </c>
+      <c r="W11" s="10">
+        <v>3.32</v>
+      </c>
+      <c r="X11" s="10">
+        <v>3.13</v>
+      </c>
+      <c r="Y11" s="10">
+        <v>3.13</v>
+      </c>
+      <c r="Z11" s="10">
+        <v>2.87</v>
+      </c>
+      <c r="AA11" s="10">
+        <v>2.66</v>
+      </c>
+      <c r="AB11" s="10">
+        <v>2.6</v>
+      </c>
+      <c r="AC11" s="10">
+        <v>2.54</v>
+      </c>
+      <c r="AD11" s="10">
+        <v>2.35</v>
+      </c>
+      <c r="AE11" s="10">
+        <v>2.19</v>
+      </c>
+      <c r="AF11" s="10">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="AG11" s="10">
+        <v>1.95</v>
+      </c>
+      <c r="AH11" s="10">
+        <v>1.64</v>
+      </c>
+      <c r="AI11" s="10">
+        <v>1.57</v>
+      </c>
+      <c r="AJ11" s="10">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AK11" s="10">
+        <v>0.94</v>
+      </c>
+      <c r="AL11" s="10">
+        <v>0.81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>